<commit_message>
:memo: Finalized the hour log. Project is ready to submit.
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Downloads/DTT Assessment - Unity - 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fcortevargas/Projects/Perfect Maze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D964BF87-5C08-B343-B443-6B031D125BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078DFF6C-36DB-7C4D-AE94-E99FE5C05EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Subject</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -79,7 +76,109 @@
     </r>
   </si>
   <si>
-    <t>Finished setting up Github repository and Unity project</t>
+    <t>Project setup</t>
+  </si>
+  <si>
+    <t>Theory familiarization</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Implemented a script that instantiates a n x m grid of cell game objects, and created very basic prefabs for the cells and walls of the maze.</t>
+  </si>
+  <si>
+    <t>Cell instantiation</t>
+  </si>
+  <si>
+    <t>Kruskal's algorithm implementation</t>
+  </si>
+  <si>
+    <t>Wall instantiation</t>
+  </si>
+  <si>
+    <t>Camera setup</t>
+  </si>
+  <si>
+    <t>Sequential maze visualization</t>
+  </si>
+  <si>
+    <t>Camera tuning</t>
+  </si>
+  <si>
+    <t>Fixed performance of large mazes by combining meshes of the border, cells and walls that won't be removed.</t>
+  </si>
+  <si>
+    <t>Performance optimization</t>
+  </si>
+  <si>
+    <t>UI setup and game manager setup</t>
+  </si>
+  <si>
+    <t>Implemented scene persistence between the maze and the main menu, and created the methods to reset and restart the maze.</t>
+  </si>
+  <si>
+    <t>Scene persistance</t>
+  </si>
+  <si>
+    <t>Fixed a bug with the camera size. It was not showing the maze properly for very wide mazes. Used https://discussions.unity.com/t/adjust-orthographic-camera-to-fit-object/130223 for reference.</t>
+  </si>
+  <si>
+    <t>Implemented the UI and game management so that user input values are not destroyed on load.</t>
+  </si>
+  <si>
+    <t>Implemented a coroutine to sequentially disable the wall game objects to generate the maze.</t>
+  </si>
+  <si>
+    <t>Wrote some code to move the camera so that it shows on the center of the screen, and to add the top, bottom, left ad right borders.</t>
+  </si>
+  <si>
+    <t>Implemented the randomized Kruskal's algorithm! Performance was an issue for a maze that is 250 by 250, but it works. Used http://weblog.jamisbuck.org/2011/1/3/maze-generation-kruskal-s-algorithm for reference.</t>
+  </si>
+  <si>
+    <t>Implemented the generation of the wall game objects at the edges of each cell game object.</t>
+  </si>
+  <si>
+    <t>Read about the Randomized Kruskal's Algorithm and understanding how to approach its implementation.</t>
+  </si>
+  <si>
+    <t>Researched about perfect maze algorithms and deciding which one I will implement. I used the wikipedia page provided on the assessment description for this.</t>
+  </si>
+  <si>
+    <t>Finished setting up Github repository and Unity project.</t>
+  </si>
+  <si>
+    <t>Fixed a bug with how the mazes were displayed. Now the camera's orthographic size is dynamically adjusted.</t>
+  </si>
+  <si>
+    <t>Camera final tuning</t>
+  </si>
+  <si>
+    <t>Tried some different things to optimize the performance (i.e. tried to used sprites instead of 3D game objects), but had no luck. Kept 3D objects with mesh combining for simplicity.</t>
+  </si>
+  <si>
+    <t>Implemented zoom and panning of the camera to make sure user can see the entire maze (works with mouse only).</t>
+  </si>
+  <si>
+    <t>Camera zooming and panning</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Created a nice game simulation in which a player can navigate the maze.</t>
+  </si>
+  <si>
+    <t>Game mode</t>
+  </si>
+  <si>
+    <t>Added comments to the scripts and wrote a README.</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Filled in the hour log and submitted.</t>
   </si>
 </sst>
 </file>
@@ -89,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -155,13 +254,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Open Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Open Sans"/>
@@ -194,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -364,6 +456,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -392,9 +495,6 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -406,22 +506,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,8 +519,26 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1696,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1705,270 +1808,410 @@
     <col min="1" max="1" width="24.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="10"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="B4" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="C6" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20">
+        <v>1.75</v>
+      </c>
+      <c r="C7" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="21">
+        <v>45317</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="21">
+        <v>45318</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="20">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="C4" s="18">
-        <v>45317</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="21">
+        <v>45318</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="23"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="20"/>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="21">
+        <v>45318</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="23"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="20"/>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="C14" s="21">
+        <v>45319</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="23"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20"/>
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="20">
+        <v>2</v>
+      </c>
+      <c r="C15" s="21">
+        <v>45319</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="23"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20"/>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="21">
+        <v>45319</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="23"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="21">
+        <v>45320</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="23"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="20"/>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="21">
+        <v>45320</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="20"/>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2.75</v>
+      </c>
+      <c r="C19" s="21">
+        <v>45320</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20"/>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="C20" s="21">
+        <v>45320</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="23"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="20"/>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="21">
+        <v>45321</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="23"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="20"/>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="20"/>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="20"/>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="20"/>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="20"/>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="20"/>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="20"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="14">
+      <c r="A30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="13">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>0.25</v>
+        <v>16.2</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1976,7 +2219,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1984,7 +2227,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1992,12 +2235,12 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>